<commit_message>
Wip(Monorepo): Icons prepared for packages
</commit_message>
<xml_diff>
--- a/_icons/prepared/iconsets-social-files-payment.xlsx
+++ b/_icons/prepared/iconsets-social-files-payment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfdrollinger/Documents/GitHub/icons/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfdrollinger/Documents/GitHub/tallui/_icons/prepared/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35272BAB-E6AE-FF48-81A5-A2B35904844C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225C8E47-5F03-FC42-A273-62F55FC5AFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="500" windowWidth="26040" windowHeight="19980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34560" yWindow="500" windowWidth="26040" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="4" r:id="rId1"/>
@@ -6505,8 +6505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17355,7 +17355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>